<commit_message>
#14: Documented ADC pinout for C2000
</commit_message>
<xml_diff>
--- a/docs/PinoutTable_v2.0.0__C2000__Breadboard_v1.0.0.xlsx
+++ b/docs/PinoutTable_v2.0.0__C2000__Breadboard_v1.0.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\SW_Projects\GestureControl\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB223AF-0E47-483C-B6F6-41FB7CC359B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527F2D67-9EDB-43B5-BC78-8AA216848199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{80607C14-953B-4F4B-8B21-B95F1610CABD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{80607C14-953B-4F4B-8B21-B95F1610CABD}"/>
   </bookViews>
   <sheets>
     <sheet name="C2000 to Breadboard Connections" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Creation Date</t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>MCP Mux Sel 2 (CD4051BE)</t>
+  </si>
+  <si>
+    <t>Power Regulator Circuit</t>
+  </si>
+  <si>
+    <t>Toggle Switch +5V</t>
+  </si>
+  <si>
+    <t>Negative Power Rail</t>
+  </si>
+  <si>
+    <t>Blue Rail</t>
+  </si>
+  <si>
+    <t>PIP Analog Mux (CD4051BE)</t>
+  </si>
+  <si>
+    <t>MCP Analog Mux (CD4051BE)</t>
   </si>
 </sst>
 </file>
@@ -780,7 +798,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,8 +900,12 @@
       <c r="D5" s="23">
         <v>21</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="24"/>
+      <c r="E5" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="G5" s="11"/>
       <c r="H5" s="21" t="s">
         <v>12</v>
@@ -910,8 +932,12 @@
       <c r="D6" s="14">
         <v>22</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="16"/>
+      <c r="E6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>17</v>
+      </c>
       <c r="G6" s="11"/>
       <c r="H6" s="21" t="s">
         <v>13</v>
@@ -1062,8 +1088,12 @@
       <c r="D12" s="14">
         <v>28</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="13">
+        <v>3</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="G12" s="11"/>
       <c r="H12" s="15"/>
       <c r="I12" s="13"/>
@@ -1110,8 +1140,12 @@
       <c r="D14" s="19">
         <v>30</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="20"/>
+      <c r="E14" s="18">
+        <v>3</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="G14" s="11"/>
       <c r="H14" s="17"/>
       <c r="I14" s="18"/>

</xml_diff>